<commit_message>
Ajout track FSATA et quelques modif pour aire fonctionner le tout
</commit_message>
<xml_diff>
--- a/02_Modèles/Lap_Time_Model/01_Simple_Model/Comparaison_Model.xlsx
+++ b/02_Modèles/Lap_Time_Model/01_Simple_Model/Comparaison_Model.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gameiro Nicolas\Documents\EPSA\Intergen\02_Modèles\Lap_Time_Model\01_Simple_Model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EPSA\Intergen\02_Modèles\Lap_Time_Model\01_Simple_Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C37CAC3C-FAFA-4B3B-A2AE-1CDB90471859}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4842545-824E-40EB-893F-0A386922533F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15400" xr2:uid="{6E2AF5FA-F89F-4AF6-A42A-943CF4481264}"/>
+    <workbookView xWindow="735" yWindow="735" windowWidth="15375" windowHeight="9390" xr2:uid="{6E2AF5FA-F89F-4AF6-A42A-943CF4481264}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -74,9 +74,6 @@
     <t>with …</t>
   </si>
   <si>
-    <t>Test_1</t>
-  </si>
-  <si>
     <t>Comparaison</t>
   </si>
   <si>
@@ -90,6 +87,9 @@
   </si>
   <si>
     <t>Concept</t>
+  </si>
+  <si>
+    <t>Test_2</t>
   </si>
 </sst>
 </file>
@@ -1803,21 +1803,21 @@
   <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="17" customWidth="1"/>
-    <col min="10" max="10" width="11.08984375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.54296875" customWidth="1"/>
-    <col min="14" max="14" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.5703125" customWidth="1"/>
+    <col min="14" max="14" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>0</v>
@@ -1825,24 +1825,24 @@
       <c r="C1" s="7"/>
       <c r="D1" s="7"/>
       <c r="E1" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F1" s="4"/>
       <c r="G1" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H1" s="5"/>
       <c r="I1" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J1" s="6"/>
       <c r="K1" s="8" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
@@ -1875,7 +1875,7 @@
       </c>
       <c r="O2" s="3"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1919,7 +1919,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1928,32 +1928,32 @@
         <v>1500</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D12" si="0">300*(($O$6*1.333/C4-1)/0.333) + 25</f>
+        <f t="shared" ref="D4:D7" si="0">300*(($O$6*1.333/C4-1)/0.333) + 25</f>
         <v>228.92792792792784</v>
       </c>
       <c r="E4">
         <v>56</v>
       </c>
       <c r="F4">
-        <f t="shared" ref="F4:F12" si="1">95.5*(($O$5*1.25/E4-1)/0.25) + 4.5</f>
+        <f t="shared" ref="F4:F7" si="1">95.5*(($O$5*1.25/E4-1)/0.25) + 4.5</f>
         <v>40.3125</v>
       </c>
       <c r="G4">
         <v>6.22</v>
       </c>
       <c r="H4">
-        <f t="shared" ref="H4:H12" si="2">71.5*((($O$4*1.5/G4)^2-1)/0.5625) + 3.5</f>
+        <f t="shared" ref="H4:H7" si="2">71.5*((($O$4*1.5/G4)^2-1)/0.5625) + 3.5</f>
         <v>53.880333352862607</v>
       </c>
       <c r="I4">
         <v>4.0599999999999996</v>
       </c>
       <c r="J4">
-        <f t="shared" ref="J4:J12" si="3">71.5*(($O$3*1.5/I4-1)/0.5) + 3.5</f>
+        <f t="shared" ref="J4:J7" si="3">71.5*(($O$3*1.5/I4-1)/0.5) + 3.5</f>
         <v>61.263546798029552</v>
       </c>
       <c r="K4">
-        <f t="shared" ref="K4:K12" si="4">D4+F4+H4+J4</f>
+        <f t="shared" ref="K4:K7" si="4">D4+F4+H4+J4</f>
         <v>384.38430807882003</v>
       </c>
       <c r="N4" t="s">
@@ -1963,7 +1963,7 @@
         <v>4.9000000000000004</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -2007,7 +2007,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -2055,42 +2055,42 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C7">
         <f>E7*120</f>
-        <v>1492.7999999999936</v>
+        <v>6841.1999999999953</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>234.25668433707489</v>
+        <v>-633.6563760743727</v>
       </c>
       <c r="E7">
-        <v>12.439999999999946</v>
+        <v>57.009999999999962</v>
       </c>
       <c r="F7">
         <f t="shared" si="1"/>
-        <v>1503.3279742765353</v>
+        <v>32.910454306262338</v>
       </c>
       <c r="G7">
-        <v>5.4499999999999282</v>
+        <v>5.4099999999999291</v>
       </c>
       <c r="H7">
         <f t="shared" si="2"/>
-        <v>107.57683603139145</v>
+        <v>111.0081501323649</v>
       </c>
       <c r="I7">
-        <v>4.4799999999999489</v>
+        <v>4.42999999999995</v>
       </c>
       <c r="J7">
         <f t="shared" si="3"/>
-        <v>42.441964285716324</v>
+        <v>44.495485327315826</v>
       </c>
       <c r="K7">
         <f t="shared" si="4"/>
-        <v>1887.6034589307178</v>
+        <v>-445.2422863084297</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
petite modif circuit, modif coeff aéro (sur rapport PAI Italien), Ajout Setup Accel pour optimus
</commit_message>
<xml_diff>
--- a/02_Modèles/Lap_Time_Model/01_Simple_Model/Comparaison_Model.xlsx
+++ b/02_Modèles/Lap_Time_Model/01_Simple_Model/Comparaison_Model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EPSA\Intergen\02_Modèles\Lap_Time_Model\01_Simple_Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4842545-824E-40EB-893F-0A386922533F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{429ED6C9-DF5C-4F4A-8BB7-0B111F4E37AA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="735" yWindow="735" windowWidth="15375" windowHeight="9390" xr2:uid="{6E2AF5FA-F89F-4AF6-A42A-943CF4481264}"/>
   </bookViews>
@@ -2061,36 +2061,36 @@
       </c>
       <c r="C7">
         <f>E7*120</f>
-        <v>6841.1999999999953</v>
+        <v>7022.3999999999951</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>-633.6563760743727</v>
+        <v>-639.90704648599365</v>
       </c>
       <c r="E7">
-        <v>57.009999999999962</v>
+        <v>58.51999999999996</v>
       </c>
       <c r="F7">
         <f t="shared" si="1"/>
-        <v>32.910454306262338</v>
+        <v>22.320574162679677</v>
       </c>
       <c r="G7">
-        <v>5.4099999999999291</v>
+        <v>5.319999999999931</v>
       </c>
       <c r="H7">
         <f t="shared" si="2"/>
-        <v>111.0081501323649</v>
+        <v>119.01354262850737</v>
       </c>
       <c r="I7">
-        <v>4.42999999999995</v>
+        <v>4.4499999999999496</v>
       </c>
       <c r="J7">
         <f t="shared" si="3"/>
-        <v>44.495485327315826</v>
+        <v>43.668539325844762</v>
       </c>
       <c r="K7">
         <f t="shared" si="4"/>
-        <v>-445.2422863084297</v>
+        <v>-454.9043903689618</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajout setup 10 pouce ( a affiner)
</commit_message>
<xml_diff>
--- a/02_Modèles/Lap_Time_Model/01_Simple_Model/Comparaison_Model.xlsx
+++ b/02_Modèles/Lap_Time_Model/01_Simple_Model/Comparaison_Model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EPSA\Intergen\02_Modèles\Lap_Time_Model\01_Simple_Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{429ED6C9-DF5C-4F4A-8BB7-0B111F4E37AA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{251A2BB4-3436-4902-BAB6-5496D4592E97}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="735" yWindow="735" windowWidth="15375" windowHeight="9390" xr2:uid="{6E2AF5FA-F89F-4AF6-A42A-943CF4481264}"/>
   </bookViews>
@@ -1803,7 +1803,7 @@
   <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2061,36 +2061,36 @@
       </c>
       <c r="C7">
         <f>E7*120</f>
-        <v>7022.3999999999951</v>
-      </c>
-      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="D7" t="e">
         <f t="shared" si="0"/>
-        <v>-639.90704648599365</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="E7">
-        <v>58.51999999999996</v>
-      </c>
-      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="F7" t="e">
         <f t="shared" si="1"/>
-        <v>22.320574162679677</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="G7">
-        <v>5.319999999999931</v>
+        <v>5.4499999999999282</v>
       </c>
       <c r="H7">
         <f t="shared" si="2"/>
-        <v>119.01354262850737</v>
+        <v>107.57683603139145</v>
       </c>
       <c r="I7">
-        <v>4.4499999999999496</v>
+        <v>4.2199999999999545</v>
       </c>
       <c r="J7">
         <f t="shared" si="3"/>
-        <v>43.668539325844762</v>
-      </c>
-      <c r="K7">
+        <v>53.651658767774585</v>
+      </c>
+      <c r="K7" t="e">
         <f t="shared" si="4"/>
-        <v>-454.9043903689618</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modif App v0.3 lancement des simulation avec button
</commit_message>
<xml_diff>
--- a/02_Modèles/Lap_Time_Model/01_Simple_Model/Comparaison_Model.xlsx
+++ b/02_Modèles/Lap_Time_Model/01_Simple_Model/Comparaison_Model.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EPSA\Intergen\02_Modèles\Lap_Time_Model\01_Simple_Model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gameiro Nicolas\Documents\EPSA\Intergen\02_Modèles\Lap_Time_Model\01_Simple_Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{429ED6C9-DF5C-4F4A-8BB7-0B111F4E37AA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{614C0CC9-FD0D-4FC8-874E-6939C04BF60A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="735" windowWidth="15375" windowHeight="9390" xr2:uid="{6E2AF5FA-F89F-4AF6-A42A-943CF4481264}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15400" xr2:uid="{6E2AF5FA-F89F-4AF6-A42A-943CF4481264}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1803,19 +1803,19 @@
   <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="17" customWidth="1"/>
-    <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.5703125" customWidth="1"/>
-    <col min="14" max="14" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.54296875" customWidth="1"/>
+    <col min="14" max="14" width="13.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>18</v>
       </c>
@@ -1840,7 +1840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>14</v>
       </c>
@@ -1875,7 +1875,7 @@
       </c>
       <c r="O2" s="3"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1919,7 +1919,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1963,7 +1963,7 @@
         <v>4.9000000000000004</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -2007,7 +2007,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -2055,7 +2055,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
Calcul des points à chaque épreuves et modification de l'appli
</commit_message>
<xml_diff>
--- a/02_Modèles/Lap_Time_Model/01_Simple_Model/Comparaison_Model.xlsx
+++ b/02_Modèles/Lap_Time_Model/01_Simple_Model/Comparaison_Model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gameiro Nicolas\Documents\EPSA\Intergen\02_Modèles\Lap_Time_Model\01_Simple_Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{614C0CC9-FD0D-4FC8-874E-6939C04BF60A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E58E2F65-4722-4869-A957-80331EC2F41C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15400" xr2:uid="{6E2AF5FA-F89F-4AF6-A42A-943CF4481264}"/>
   </bookViews>
@@ -1803,7 +1803,7 @@
   <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>